<commit_message>
Mejoras y nuevos mockup
Mejoras a diseños de mockups de interfaces, y creación de mockup de las vistas de clientes, nuevo cliente y editar cliente
</commit_message>
<xml_diff>
--- a/Nana&Rene/MateriasPrimas.xlsx
+++ b/Nana&Rene/MateriasPrimas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
@@ -20,7 +20,7 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>harina</t>
+    <t>harinita</t>
   </si>
   <si>
     <t>manzana</t>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>leche</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -175,6 +178,14 @@
         <v>8.0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Arreglo errores interfaz gráfica
</commit_message>
<xml_diff>
--- a/Nana&Rene/MateriasPrimas.xlsx
+++ b/Nana&Rene/MateriasPrimas.xlsx
@@ -111,7 +111,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="3">
@@ -127,7 +127,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="5">
@@ -167,7 +167,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -175,7 +175,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
materia prima (tipo), validación cant materia prima
</commit_message>
<xml_diff>
--- a/Nana&Rene/MateriasPrimas.xlsx
+++ b/Nana&Rene/MateriasPrimas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Nombre</t>
   </si>
@@ -20,9 +20,15 @@
     <t>Cantidad</t>
   </si>
   <si>
+    <t>Tipo</t>
+  </si>
+  <si>
     <t>harinita</t>
   </si>
   <si>
+    <t>discreta</t>
+  </si>
+  <si>
     <t>manzana</t>
   </si>
   <si>
@@ -48,6 +54,15 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>pelo de vaca</t>
+  </si>
+  <si>
+    <t>pelo de cerdo</t>
+  </si>
+  <si>
+    <t>continua</t>
   </si>
 </sst>
 </file>
@@ -105,85 +120,140 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
         <v>10.0</v>
       </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
         <v>30.0</v>
       </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
         <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
         <v>5.0</v>
       </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
         <v>2.0</v>
       </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
         <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
         <v>8.0</v>
       </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
         <v>12.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Historial de pedidos de un cliente
</commit_message>
<xml_diff>
--- a/Nana&Rene/MateriasPrimas.xlsx
+++ b/Nana&Rene/MateriasPrimas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>Pelo de vaca</t>
   </si>
   <si>
     <t>Pelo de cerdo</t>
@@ -217,7 +214,7 @@
         <v>12.0</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -225,20 +222,9 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>12.0</v>
+        <v>30.0</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="C12" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>